<commit_message>
latest working version. all median planes defined
</commit_message>
<xml_diff>
--- a/ribs_checklist.xlsx
+++ b/ribs_checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIPAG_~1\AppData\Local\Temp\Mxt214\RemoteFiles\133316_2_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIPAG_~1\AppData\Local\Temp\Mxt214\RemoteFiles\66984_3_58\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="121">
   <si>
     <t>Cohort</t>
   </si>
@@ -290,12 +290,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Insp</t>
-  </si>
-  <si>
-    <t>EESupine</t>
-  </si>
-  <si>
     <t>AGING004</t>
   </si>
   <si>
@@ -320,9 +314,6 @@
     <t>DICOMs?</t>
   </si>
   <si>
-    <t>FRC</t>
-  </si>
-  <si>
     <t>DICOM Location</t>
   </si>
   <si>
@@ -333,9 +324,6 @@
   </si>
   <si>
     <t>Expn</t>
-  </si>
-  <si>
-    <t>/eresearch/lung/mpag253/Archive</t>
   </si>
   <si>
     <t>/hpc/mpag253/Torso/segmentation</t>
@@ -404,13 +392,16 @@
     <t>*still very poor, alt directions, lung proximity, threshold?</t>
   </si>
   <si>
-    <t>*very crap</t>
-  </si>
-  <si>
     <t>*11 ribs</t>
   </si>
   <si>
     <t>EEsupine</t>
+  </si>
+  <si>
+    <t>*very crap - fix nifti file</t>
+  </si>
+  <si>
+    <t>OMIT</t>
   </si>
 </sst>
 </file>
@@ -529,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -662,7 +653,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -670,157 +673,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="58">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="43">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1573,11 +1426,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F74" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="M130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D85" sqref="D85"/>
+      <selection pane="bottomRight" activeCell="A153" sqref="A153:A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,49 +1467,49 @@
         <v>1</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F1" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="I1" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="R1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="37" t="s">
         <v>112</v>
-      </c>
-      <c r="S1" s="37" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1670,7 +1523,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F2" s="32">
         <v>768</v>
@@ -1718,7 +1571,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F3" s="32">
         <v>768</v>
@@ -1766,7 +1619,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F4" s="32">
         <v>768</v>
@@ -1808,13 +1661,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F5" s="32">
         <v>768</v>
@@ -1862,7 +1715,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F6" s="32">
         <v>768</v>
@@ -1910,7 +1763,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F7" s="32">
         <v>768</v>
@@ -1952,13 +1805,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F8" s="32">
         <v>768</v>
@@ -2007,7 +1860,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F9" s="32">
         <v>768</v>
@@ -2055,7 +1908,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F10" s="32">
         <v>768</v>
@@ -2103,7 +1956,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F11" s="32">
         <v>768</v>
@@ -2151,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F12" s="32">
         <v>768</v>
@@ -2178,11 +2031,11 @@
         <v>2</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="R12" s="6"/>
       <c r="S12" s="46" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2196,7 +2049,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F13" s="32">
         <v>768</v>
@@ -2244,7 +2097,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F14" s="32">
         <v>768</v>
@@ -2293,7 +2146,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F15" s="32">
         <v>768</v>
@@ -2342,7 +2195,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F16" s="32">
         <v>768</v>
@@ -2391,7 +2244,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F17" s="32">
         <v>768</v>
@@ -2439,7 +2292,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F18" s="32">
         <v>768</v>
@@ -2487,7 +2340,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F19" s="32">
         <v>768</v>
@@ -2535,7 +2388,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F20" s="32">
         <v>768</v>
@@ -2583,7 +2436,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F21" s="32">
         <v>768</v>
@@ -2620,7 +2473,7 @@
       </c>
       <c r="R21" s="6"/>
       <c r="S21" s="39" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -2634,7 +2487,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F22" s="32">
         <v>768</v>
@@ -2682,7 +2535,7 @@
         <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F23" s="32">
         <v>768</v>
@@ -2730,7 +2583,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F24" s="32">
         <v>768</v>
@@ -2778,7 +2631,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F25" s="32">
         <v>768</v>
@@ -2826,7 +2679,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F26" s="32">
         <v>768</v>
@@ -2875,7 +2728,7 @@
         <v>3</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F27" s="32">
         <v>768</v>
@@ -2923,7 +2776,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F28" s="32">
         <v>768</v>
@@ -2967,11 +2820,11 @@
       <c r="C29" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>85</v>
+      <c r="D29" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F29" s="32">
         <v>768</v>
@@ -3014,13 +2867,13 @@
         <v>4</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F30" s="32">
         <v>768</v>
@@ -3068,7 +2921,7 @@
         <v>3</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F31" s="32">
         <v>768</v>
@@ -3116,7 +2969,7 @@
         <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F32" s="32">
         <v>768</v>
@@ -3164,7 +3017,7 @@
         <v>3</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F33" s="32">
         <v>768</v>
@@ -3208,11 +3061,11 @@
       <c r="C34" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>85</v>
+      <c r="D34" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F34" s="32">
         <v>768</v>
@@ -3256,11 +3109,11 @@
       <c r="C35" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>85</v>
+      <c r="D35" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F35" s="32">
         <v>768</v>
@@ -3308,7 +3161,7 @@
         <v>3</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F36" s="32">
         <v>768</v>
@@ -3356,7 +3209,7 @@
         <v>3</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F37" s="32">
         <v>768</v>
@@ -3404,7 +3257,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F38" s="32">
         <v>768</v>
@@ -3452,7 +3305,7 @@
         <v>3</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F39" s="32">
         <v>768</v>
@@ -3494,13 +3347,13 @@
         <v>4</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="D40" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F40" s="32">
         <v>768</v>
@@ -3542,13 +3395,13 @@
         <v>4</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="D41" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F41" s="32">
         <v>512</v>
@@ -3575,11 +3428,11 @@
         <v>2</v>
       </c>
       <c r="O41" s="20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="R41" s="6"/>
       <c r="S41" s="46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -3589,11 +3442,11 @@
       <c r="C42" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="17" t="s">
-        <v>85</v>
+      <c r="D42" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F42" s="32">
         <v>768</v>
@@ -3637,11 +3490,11 @@
       <c r="C43" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="17" t="s">
-        <v>85</v>
+      <c r="D43" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F43" s="32">
         <v>768</v>
@@ -3683,13 +3536,13 @@
         <v>4</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="D44" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F44" s="32">
         <v>512</v>
@@ -3733,11 +3586,11 @@
       <c r="C45" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="17" t="s">
-        <v>85</v>
+      <c r="D45" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F45" s="32">
         <v>512</v>
@@ -3781,11 +3634,11 @@
       <c r="C46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="17" t="s">
-        <v>85</v>
+      <c r="D46" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F46" s="32">
         <v>512</v>
@@ -3829,11 +3682,11 @@
       <c r="C47" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="17" t="s">
-        <v>85</v>
+      <c r="D47" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F47" s="32">
         <v>512</v>
@@ -3879,10 +3732,10 @@
         <v>41</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F48" s="32">
         <v>512</v>
@@ -3932,7 +3785,7 @@
         <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F49" s="32">
         <v>512</v>
@@ -3959,11 +3812,11 @@
         <v>2</v>
       </c>
       <c r="O49" s="20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="R49" s="20"/>
       <c r="S49" s="46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -3977,7 +3830,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F50" s="32">
         <v>512</v>
@@ -4025,7 +3878,7 @@
         <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F51" s="32">
         <v>512</v>
@@ -4062,7 +3915,7 @@
       </c>
       <c r="R51" s="6"/>
       <c r="S51" s="43" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
@@ -4076,7 +3929,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F52" s="32">
         <v>512</v>
@@ -4124,7 +3977,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F53" s="32">
         <v>512</v>
@@ -4172,7 +4025,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F54" s="32">
         <v>512</v>
@@ -4220,7 +4073,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F55" s="32">
         <v>512</v>
@@ -4269,7 +4122,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F56" s="32">
         <v>512</v>
@@ -4318,7 +4171,7 @@
         <v>3</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F57" s="32">
         <v>512</v>
@@ -4368,7 +4221,7 @@
         <v>3</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F58" s="32">
         <v>512</v>
@@ -4417,7 +4270,7 @@
         <v>3</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F59" s="32">
         <v>512</v>
@@ -4454,7 +4307,7 @@
       </c>
       <c r="R59" s="6"/>
       <c r="S59" s="43" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
@@ -4468,7 +4321,7 @@
         <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F60" s="32">
         <v>512</v>
@@ -4517,7 +4370,7 @@
         <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F61" s="32">
         <v>512</v>
@@ -4565,7 +4418,7 @@
         <v>3</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F62" s="32">
         <v>512</v>
@@ -4614,7 +4467,7 @@
         <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F63" s="32">
         <v>512</v>
@@ -4663,7 +4516,7 @@
         <v>3</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F64" s="32">
         <v>512</v>
@@ -4713,7 +4566,7 @@
         <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F65" s="32">
         <v>512</v>
@@ -4762,7 +4615,7 @@
         <v>3</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F66" s="32">
         <v>512</v>
@@ -4810,7 +4663,7 @@
         <v>3</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F67" s="32">
         <v>512</v>
@@ -4858,7 +4711,7 @@
         <v>3</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F68" s="32">
         <v>512</v>
@@ -4906,7 +4759,7 @@
         <v>3</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F69" s="32">
         <v>512</v>
@@ -4954,7 +4807,7 @@
         <v>3</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F70" s="32">
         <v>512</v>
@@ -5002,7 +4855,7 @@
         <v>3</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F71" s="32">
         <v>512</v>
@@ -5050,7 +4903,7 @@
         <v>3</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F72" s="32">
         <v>512</v>
@@ -5098,7 +4951,7 @@
         <v>3</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F73" s="32">
         <v>512</v>
@@ -5146,7 +4999,7 @@
         <v>3</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F74" s="32">
         <v>512</v>
@@ -5194,7 +5047,7 @@
         <v>3</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F75" s="32">
         <v>512</v>
@@ -5242,7 +5095,7 @@
         <v>3</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F76" s="32">
         <v>512</v>
@@ -5290,7 +5143,7 @@
         <v>3</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F77" s="32">
         <v>512</v>
@@ -5338,7 +5191,7 @@
         <v>3</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F78" s="32">
         <v>512</v>
@@ -5386,7 +5239,7 @@
         <v>3</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F79" s="32">
         <v>512</v>
@@ -5434,7 +5287,7 @@
         <v>3</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F80" s="32">
         <v>512</v>
@@ -5482,7 +5335,7 @@
         <v>3</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F81" s="32">
         <v>512</v>
@@ -5530,7 +5383,7 @@
         <v>3</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F82" s="32">
         <v>512</v>
@@ -5579,7 +5432,7 @@
         <v>3</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F83" s="32">
         <v>512</v>
@@ -5617,7 +5470,7 @@
       </c>
       <c r="R83" s="20"/>
       <c r="S83" s="42" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5626,13 +5479,13 @@
         <v>5</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D84" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E84" s="21" t="s">
         <v>97</v>
-      </c>
-      <c r="E84" s="21" t="s">
-        <v>101</v>
       </c>
       <c r="F84" s="34">
         <v>512</v>
@@ -5670,13 +5523,10 @@
       </c>
       <c r="R84" s="3"/>
       <c r="S84" s="40" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>1</v>
-      </c>
       <c r="B85" t="s">
         <v>4</v>
       </c>
@@ -5684,10 +5534,10 @@
         <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F85" s="32">
         <v>768</v>
@@ -5720,10 +5570,10 @@
         <v>8</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F86" s="32">
         <v>768</v>
@@ -5756,10 +5606,10 @@
         <v>9</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F87" s="32">
         <v>768</v>
@@ -5789,13 +5639,13 @@
         <v>4</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F88" s="32">
         <v>768</v>
@@ -5828,10 +5678,10 @@
         <v>10</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F89" s="32">
         <v>768</v>
@@ -5864,7 +5714,7 @@
         <v>11</v>
       </c>
       <c r="D90" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E90" s="8"/>
       <c r="I90" s="33"/>
@@ -5880,13 +5730,13 @@
         <v>4</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F91" s="32">
         <v>768</v>
@@ -5919,10 +5769,10 @@
         <v>12</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E92" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F92" s="32">
         <v>768</v>
@@ -5955,10 +5805,10 @@
         <v>13</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F93" s="32">
         <v>768</v>
@@ -5991,10 +5841,10 @@
         <v>14</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F94" s="32">
         <v>768</v>
@@ -6027,10 +5877,10 @@
         <v>15</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E95" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F95" s="32">
         <v>768</v>
@@ -6063,10 +5913,10 @@
         <v>16</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E96" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F96" s="32">
         <v>768</v>
@@ -6099,10 +5949,10 @@
         <v>17</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E97" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F97" s="32">
         <v>768</v>
@@ -6135,10 +5985,10 @@
         <v>18</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E98" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F98" s="32">
         <v>768</v>
@@ -6171,10 +6021,10 @@
         <v>19</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F99" s="32">
         <v>768</v>
@@ -6207,10 +6057,10 @@
         <v>20</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F100" s="32">
         <v>768</v>
@@ -6243,10 +6093,10 @@
         <v>21</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E101" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F101" s="32">
         <v>768</v>
@@ -6279,10 +6129,10 @@
         <v>22</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E102" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F102" s="32">
         <v>768</v>
@@ -6315,10 +6165,10 @@
         <v>23</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E103" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F103" s="32">
         <v>768</v>
@@ -6351,10 +6201,10 @@
         <v>24</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E104" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F104" s="32">
         <v>768</v>
@@ -6387,10 +6237,10 @@
         <v>25</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E105" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F105" s="32">
         <v>768</v>
@@ -6423,10 +6273,10 @@
         <v>26</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E106" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F106" s="32">
         <v>768</v>
@@ -6459,10 +6309,10 @@
         <v>27</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E107" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F107" s="32">
         <v>768</v>
@@ -6495,10 +6345,10 @@
         <v>28</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E108" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F108" s="32">
         <v>768</v>
@@ -6531,10 +6381,10 @@
         <v>29</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E109" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F109" s="32">
         <v>768</v>
@@ -6567,10 +6417,10 @@
         <v>30</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E110" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F110" s="32">
         <v>768</v>
@@ -6603,10 +6453,10 @@
         <v>31</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E111" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F111" s="32">
         <v>768</v>
@@ -6639,10 +6489,10 @@
         <v>32</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E112" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F112" s="32">
         <v>768</v>
@@ -6672,13 +6522,13 @@
         <v>4</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E113" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F113" s="32">
         <v>768</v>
@@ -6711,10 +6561,10 @@
         <v>33</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E114" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F114" s="32">
         <v>768</v>
@@ -6747,10 +6597,10 @@
         <v>34</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E115" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F115" s="32">
         <v>768</v>
@@ -6783,10 +6633,10 @@
         <v>35</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E116" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F116" s="32">
         <v>768</v>
@@ -6819,10 +6669,10 @@
         <v>36</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E117" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F117" s="32">
         <v>768</v>
@@ -6855,10 +6705,10 @@
         <v>37</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E118" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F118" s="32">
         <v>768</v>
@@ -6891,10 +6741,10 @@
         <v>42</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E119" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F119" s="32">
         <v>768</v>
@@ -6927,10 +6777,10 @@
         <v>38</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E120" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F120" s="32">
         <v>768</v>
@@ -6963,10 +6813,10 @@
         <v>43</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E121" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F121" s="32">
         <v>768</v>
@@ -6999,10 +6849,10 @@
         <v>44</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E122" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F122" s="32">
         <v>768</v>
@@ -7032,13 +6882,13 @@
         <v>4</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E123" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F123" s="32">
         <v>768</v>
@@ -7068,13 +6918,13 @@
         <v>4</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E124" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F124" s="32">
         <v>768</v>
@@ -7107,10 +6957,10 @@
         <v>45</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E125" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F125" s="32">
         <v>768</v>
@@ -7143,10 +6993,10 @@
         <v>46</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E126" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F126" s="32">
         <v>768</v>
@@ -7176,13 +7026,13 @@
         <v>4</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E127" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F127" s="32">
         <v>512</v>
@@ -7215,10 +7065,10 @@
         <v>39</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E128" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F128" s="32">
         <v>512</v>
@@ -7251,10 +7101,10 @@
         <v>40</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E129" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F129" s="32">
         <v>512</v>
@@ -7287,10 +7137,10 @@
         <v>47</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E130" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F130" s="32">
         <v>512</v>
@@ -7324,10 +7174,10 @@
         <v>41</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E131" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F131" s="32">
         <v>512</v>
@@ -7366,13 +7216,13 @@
         <v>48</v>
       </c>
       <c r="D132" s="16" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="I132" s="33"/>
       <c r="J132" s="33"/>
       <c r="K132" s="33"/>
-      <c r="M132" s="6" t="s">
-        <v>84</v>
+      <c r="M132" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="R132" s="6"/>
     </row>
@@ -7384,10 +7234,10 @@
         <v>49</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E133" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F133" s="32">
         <v>512</v>
@@ -7410,6 +7260,9 @@
       <c r="M133" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N133" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R133" s="6"/>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
@@ -7420,10 +7273,10 @@
         <v>50</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E134" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F134" s="32">
         <v>512</v>
@@ -7446,6 +7299,9 @@
       <c r="M134" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N134" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R134" s="6"/>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
@@ -7456,10 +7312,10 @@
         <v>51</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E135" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F135" s="32">
         <v>512</v>
@@ -7482,6 +7338,9 @@
       <c r="M135" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N135" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R135" s="6"/>
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
@@ -7492,10 +7351,10 @@
         <v>52</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E136" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F136" s="32">
         <v>512</v>
@@ -7518,6 +7377,9 @@
       <c r="M136" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N136" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R136" s="6"/>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
@@ -7528,10 +7390,10 @@
         <v>53</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E137" s="14" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="E137" s="52" t="s">
+        <v>97</v>
       </c>
       <c r="F137" s="32">
         <v>512</v>
@@ -7554,6 +7416,9 @@
       <c r="M137" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N137" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R137" s="6"/>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
@@ -7564,10 +7429,10 @@
         <v>54</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E138" s="14" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="E138" s="52" t="s">
+        <v>97</v>
       </c>
       <c r="F138" s="32">
         <v>512</v>
@@ -7590,6 +7455,9 @@
       <c r="M138" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N138" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R138" s="6"/>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
@@ -7600,10 +7468,10 @@
         <v>55</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E139" s="14" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="E139" s="52" t="s">
+        <v>97</v>
       </c>
       <c r="F139" s="32">
         <v>512</v>
@@ -7626,6 +7494,9 @@
       <c r="M139" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N139" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R139" s="6"/>
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
@@ -7636,10 +7507,10 @@
         <v>56</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E140" s="14" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="E140" s="52" t="s">
+        <v>97</v>
       </c>
       <c r="F140" s="32">
         <v>512</v>
@@ -7662,6 +7533,9 @@
       <c r="M140" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N140" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R140" s="6"/>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
@@ -7672,10 +7546,10 @@
         <v>57</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E141" s="8" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E141" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F141" s="32">
         <v>512</v>
@@ -7698,6 +7572,9 @@
       <c r="M141" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N141" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R141" s="6"/>
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.25">
@@ -7708,10 +7585,10 @@
         <v>58</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E142" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F142" s="32">
         <v>512</v>
@@ -7734,6 +7611,9 @@
       <c r="M142" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N142" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R142" s="6"/>
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.25">
@@ -7744,10 +7624,10 @@
         <v>59</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E143" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F143" s="32">
         <v>512</v>
@@ -7770,6 +7650,9 @@
       <c r="M143" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N143" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R143" s="6"/>
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
@@ -7780,10 +7663,10 @@
         <v>60</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E144" s="14" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="E144" s="52" t="s">
+        <v>97</v>
       </c>
       <c r="F144" s="32">
         <v>512</v>
@@ -7806,9 +7689,12 @@
       <c r="M144" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N144" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R144" s="6"/>
     </row>
-    <row r="145" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>5</v>
       </c>
@@ -7816,10 +7702,10 @@
         <v>61</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E145" s="8" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E145" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F145" s="32">
         <v>512</v>
@@ -7842,9 +7728,12 @@
       <c r="M145" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N145" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R145" s="6"/>
     </row>
-    <row r="146" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>5</v>
       </c>
@@ -7852,10 +7741,10 @@
         <v>62</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E146" s="14" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="E146" s="52" t="s">
+        <v>97</v>
       </c>
       <c r="F146" s="32">
         <v>512</v>
@@ -7878,27 +7767,54 @@
       <c r="M146" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N146" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R146" s="6"/>
     </row>
-    <row r="147" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>1</v>
+      </c>
       <c r="B147" t="s">
         <v>5</v>
       </c>
-      <c r="C147" s="16" t="s">
+      <c r="C147" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D147" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="I147" s="33"/>
-      <c r="J147" s="33"/>
-      <c r="K147" s="33"/>
+      <c r="D147" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E147" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="F147" s="32">
+        <v>512</v>
+      </c>
+      <c r="G147" s="32">
+        <v>512</v>
+      </c>
+      <c r="H147" s="32">
+        <v>644</v>
+      </c>
+      <c r="I147" s="33">
+        <v>0.5078125</v>
+      </c>
+      <c r="J147" s="33">
+        <v>0.5078125</v>
+      </c>
+      <c r="K147" s="33">
+        <v>0.5</v>
+      </c>
       <c r="M147" s="6" t="s">
-        <v>84</v>
+        <v>2</v>
+      </c>
+      <c r="N147" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="R147" s="6"/>
     </row>
-    <row r="148" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>5</v>
       </c>
@@ -7906,10 +7822,10 @@
         <v>64</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E148" s="14" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="E148" s="52" t="s">
+        <v>97</v>
       </c>
       <c r="F148" s="32">
         <v>512</v>
@@ -7932,9 +7848,12 @@
       <c r="M148" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N148" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R148" s="6"/>
     </row>
-    <row r="149" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>5</v>
       </c>
@@ -7942,10 +7861,10 @@
         <v>65</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E149" s="8" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E149" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F149" s="32">
         <v>512</v>
@@ -7968,9 +7887,12 @@
       <c r="M149" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N149" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R149" s="6"/>
     </row>
-    <row r="150" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>5</v>
       </c>
@@ -7978,10 +7900,10 @@
         <v>66</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E150" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F150" s="32">
         <v>512</v>
@@ -8004,9 +7926,12 @@
       <c r="M150" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N150" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R150" s="6"/>
     </row>
-    <row r="151" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>5</v>
       </c>
@@ -8014,8 +7939,9 @@
         <v>67</v>
       </c>
       <c r="D151" s="16" t="s">
-        <v>86</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E151" s="51"/>
       <c r="I151" s="33"/>
       <c r="J151" s="33"/>
       <c r="K151" s="33"/>
@@ -8024,7 +7950,7 @@
       </c>
       <c r="R151" s="6"/>
     </row>
-    <row r="152" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>5</v>
       </c>
@@ -8032,10 +7958,10 @@
         <v>68</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E152" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F152" s="32">
         <v>512</v>
@@ -8058,9 +7984,12 @@
       <c r="M152" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N152" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R152" s="6"/>
     </row>
-    <row r="153" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>5</v>
       </c>
@@ -8068,10 +7997,10 @@
         <v>69</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E153" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F153" s="32">
         <v>512</v>
@@ -8094,20 +8023,23 @@
       <c r="M153" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N153" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R153" s="6"/>
     </row>
-    <row r="154" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>5</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D154" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E154" s="14" t="s">
-        <v>101</v>
+      <c r="D154" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E154" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F154" s="32">
         <v>512</v>
@@ -8130,20 +8062,23 @@
       <c r="M154" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N154" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R154" s="6"/>
     </row>
-    <row r="155" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>5</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D155" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>100</v>
+      <c r="D155" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E155" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F155" s="32">
         <v>512</v>
@@ -8166,20 +8101,23 @@
       <c r="M155" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N155" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R155" s="6"/>
     </row>
-    <row r="156" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>5</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D156" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>100</v>
+      <c r="D156" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E156" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F156" s="32">
         <v>512</v>
@@ -8202,20 +8140,23 @@
       <c r="M156" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N156" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R156" s="6"/>
     </row>
-    <row r="157" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>5</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D157" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E157" s="14" t="s">
-        <v>101</v>
+      <c r="D157" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E157" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F157" s="32">
         <v>512</v>
@@ -8238,20 +8179,23 @@
       <c r="M157" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N157" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R157" s="6"/>
     </row>
-    <row r="158" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>5</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D158" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>100</v>
+      <c r="D158" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E158" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F158" s="32">
         <v>512</v>
@@ -8274,20 +8218,23 @@
       <c r="M158" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N158" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R158" s="6"/>
     </row>
-    <row r="159" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>5</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D159" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>100</v>
+      <c r="D159" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E159" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F159" s="32">
         <v>512</v>
@@ -8310,20 +8257,23 @@
       <c r="M159" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N159" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R159" s="6"/>
     </row>
-    <row r="160" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>5</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D160" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>100</v>
+      <c r="D160" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E160" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F160" s="32">
         <v>512</v>
@@ -8346,6 +8296,9 @@
       <c r="M160" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N160" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R160" s="6"/>
     </row>
     <row r="161" spans="2:18" x14ac:dyDescent="0.25">
@@ -8355,11 +8308,11 @@
       <c r="C161" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D161" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>100</v>
+      <c r="D161" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E161" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F161" s="32">
         <v>512</v>
@@ -8382,6 +8335,9 @@
       <c r="M161" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N161" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R161" s="6"/>
     </row>
     <row r="162" spans="2:18" x14ac:dyDescent="0.25">
@@ -8391,11 +8347,11 @@
       <c r="C162" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D162" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>100</v>
+      <c r="D162" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E162" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="F162" s="32">
         <v>512</v>
@@ -8418,6 +8374,9 @@
       <c r="M162" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N162" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R162" s="6"/>
     </row>
     <row r="163" spans="2:18" x14ac:dyDescent="0.25">
@@ -8427,11 +8386,11 @@
       <c r="C163" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D163" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E163" s="14" t="s">
-        <v>101</v>
+      <c r="D163" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E163" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="F163" s="32">
         <v>512</v>
@@ -8454,6 +8413,9 @@
       <c r="M163" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N163" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R163" s="6"/>
     </row>
     <row r="164" spans="2:18" x14ac:dyDescent="0.25">
@@ -8464,10 +8426,10 @@
         <v>80</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E164" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="F164" s="32">
         <v>512</v>
@@ -8490,6 +8452,9 @@
       <c r="M164" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N164" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R164" s="6"/>
     </row>
     <row r="165" spans="2:18" x14ac:dyDescent="0.25">
@@ -8500,10 +8465,10 @@
         <v>81</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E165" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="F165" s="32">
         <v>512</v>
@@ -8526,6 +8491,9 @@
       <c r="M165" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N165" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R165" s="6"/>
     </row>
     <row r="166" spans="2:18" x14ac:dyDescent="0.25">
@@ -8536,10 +8504,10 @@
         <v>82</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="E166" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="F166" s="32">
         <v>512</v>
@@ -8562,6 +8530,9 @@
       <c r="M166" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N166" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R166" s="6"/>
     </row>
     <row r="167" spans="2:18" x14ac:dyDescent="0.25">
@@ -8569,13 +8540,13 @@
         <v>5</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E167" s="14" t="s">
-        <v>101</v>
+        <v>91</v>
+      </c>
+      <c r="D167" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E167" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="F167" s="32">
         <v>512</v>
@@ -8598,211 +8569,219 @@
       <c r="M167" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="N167" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="R167" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="N137:N140 N144 N146 N148 N154 N157 N163 N49 P49:Q49 N141:R143 N164:R1048576 N158:R162 N155:R156 N152:R153 N149:R150 N145:R145 N133:R136 R71 N85:Q131 R84:R131 P66:R70 N50:R50 N51:O62 N66:O84 S21 S8 S26 N1:R48 P51:R56 P57:Q57 P58:R62 N63:R65 P72:R83">
-    <cfRule type="cellIs" dxfId="57" priority="339" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="341" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M72">
-    <cfRule type="cellIs" dxfId="56" priority="266" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="268" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M73">
-    <cfRule type="cellIs" dxfId="55" priority="262" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="264" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M3">
-    <cfRule type="cellIs" dxfId="54" priority="307" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="309" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:M7 M9:M48">
-    <cfRule type="cellIs" dxfId="53" priority="306" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="308" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M66">
-    <cfRule type="cellIs" dxfId="52" priority="298" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="300" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M67">
-    <cfRule type="cellIs" dxfId="51" priority="294" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="296" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="cellIs" dxfId="50" priority="293" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="295" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M69">
-    <cfRule type="cellIs" dxfId="49" priority="290" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="292" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M71">
-    <cfRule type="cellIs" dxfId="48" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="284" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M74">
-    <cfRule type="cellIs" dxfId="47" priority="280" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="282" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M77">
-    <cfRule type="cellIs" dxfId="46" priority="278" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="280" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M78">
-    <cfRule type="cellIs" dxfId="45" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="278" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M80">
-    <cfRule type="cellIs" dxfId="44" priority="274" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="276" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M70">
-    <cfRule type="cellIs" dxfId="43" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="272" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="cellIs" dxfId="42" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="219" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M75">
-    <cfRule type="cellIs" dxfId="41" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="260" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M76">
-    <cfRule type="cellIs" dxfId="40" priority="254" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="256" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M79">
-    <cfRule type="cellIs" dxfId="39" priority="250" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="252" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M81">
-    <cfRule type="cellIs" dxfId="38" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="248" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M82">
-    <cfRule type="cellIs" dxfId="37" priority="244" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="246" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M83:M84">
-    <cfRule type="cellIs" dxfId="36" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="242" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M91:M131 M85:M89">
-    <cfRule type="cellIs" dxfId="35" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="150" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N147:Q147 O146:Q146 O148:Q148 R146:R148 O163:R163 O157:R157 O154:R154 N151:R151 O144:R144 O137:R140 N132:R132">
-    <cfRule type="cellIs" dxfId="34" priority="142" operator="equal">
+  <conditionalFormatting sqref="O146:R148 O163:R163 O157:R157 O154:R154 N151:R151 O144:R144 O137:R140 N132:R132">
+    <cfRule type="cellIs" dxfId="19" priority="144" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M132">
-    <cfRule type="cellIs" dxfId="33" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="122" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M133">
-    <cfRule type="cellIs" dxfId="32" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="119" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M134:M146 M148:M150 M152:M167">
-    <cfRule type="cellIs" dxfId="31" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="99" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M151">
-    <cfRule type="cellIs" dxfId="30" priority="77" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M147">
-    <cfRule type="cellIs" dxfId="29" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="79" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28">
-    <cfRule type="cellIs" dxfId="28" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="56" operator="equal">
       <formula>"oldformat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29:M48">
-    <cfRule type="cellIs" dxfId="27" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="55" operator="equal">
       <formula>"oldformat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="26" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="46" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="cellIs" dxfId="25" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="44" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M90">
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="32" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P84">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="25" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P71:Q71">
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="24" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R49">
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R57">
-    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14:S16">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q84">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M147">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N147">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>